<commit_message>
Updated counter PLL calculator
</commit_message>
<xml_diff>
--- a/Docs/Other/Counter_PLL_Calc.xlsx
+++ b/Docs/Other/Counter_PLL_Calc.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18311"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unkno\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04D44088-EFB9-4879-922C-E7518C8E3E94}" xr6:coauthVersionLast="20" xr6:coauthVersionMax="20" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Counter PLL Calc" sheetId="1" r:id="rId1"/>
     <sheet name="REF" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171026"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+  <si>
+    <t>PLLDIV dividers</t>
+  </si>
   <si>
     <t>VCO/1</t>
   </si>
@@ -51,40 +55,40 @@
     <t>VCO/128</t>
   </si>
   <si>
+    <t>min/max PLL_in</t>
+  </si>
+  <si>
+    <t>Enter desired counter output frequency</t>
+  </si>
+  <si>
+    <t>PLL_out =</t>
+  </si>
+  <si>
     <t>Hz</t>
   </si>
   <si>
+    <t>Enter system clock frequency</t>
+  </si>
+  <si>
+    <t>CLK_FREQ =</t>
+  </si>
+  <si>
+    <t>RESULTS</t>
+  </si>
+  <si>
+    <t>PLLDIV =</t>
+  </si>
+  <si>
     <t>x VCO</t>
   </si>
   <si>
-    <t>PLL_out =</t>
-  </si>
-  <si>
-    <t>PLLDIV =</t>
-  </si>
-  <si>
-    <t>CLK_FREQ =</t>
-  </si>
-  <si>
-    <t>PLL_in =</t>
-  </si>
-  <si>
     <t>FRQX =</t>
   </si>
   <si>
-    <t>min/max PLL_in</t>
-  </si>
-  <si>
-    <t>PLLDIV dividers</t>
+    <t>(decimal)</t>
   </si>
   <si>
     <t>=</t>
-  </si>
-  <si>
-    <t>CALCULATE</t>
-  </si>
-  <si>
-    <t>(decimal)</t>
   </si>
   <si>
     <t>(binary)</t>
@@ -96,11 +100,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="#\ ???/???"/>
+    <numFmt numFmtId="164" formatCode="#\ ???/???"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +132,14 @@
       <color rgb="FF333333"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -393,47 +405,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -452,35 +434,62 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -761,16 +770,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -784,248 +793,237 @@
     <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="3"/>
-      <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="C2" s="19" t="s">
+    <row r="1" spans="1:11">
+      <c r="B1" s="1"/>
+      <c r="C1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1"/>
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="D2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="F2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="H2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="I2" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="17" t="str">
+      <c r="J2" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="43.5" customHeight="1">
+      <c r="A3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7" t="str">
         <f>IF(REF!B3&gt;=10^6,TEXT(REF!B3/10^6,"0.0#")&amp;" MHz",IF(REF!B3&gt;=10^3,TEXT(REF!B3/10^3,"0.0#")&amp;" KHz",TEXT(REF!B3,"0.0#")&amp;" Hz"))</f>
         <v>4.0 MHz</v>
       </c>
-      <c r="C3" s="5" t="str">
+      <c r="C3" s="2" t="str">
         <f>IF(REF!C3&gt;=10^6,TEXT(REF!C3/10^6,"0.0#")&amp;" MHz",IF(REF!C3&gt;=10^3,TEXT(REF!C3/10^3,"0.0#")&amp;" KHz",TEXT(REF!C3,"0.0#")&amp;" Hz"))</f>
         <v>64.0 MHz</v>
       </c>
-      <c r="D3" s="5" t="str">
+      <c r="D3" s="2" t="str">
         <f>IF(REF!D3&gt;=10^6,TEXT(REF!D3/10^6,"0.0#")&amp;" MHz",IF(REF!D3&gt;=10^3,TEXT(REF!D3/10^3,"0.0#")&amp;" KHz",TEXT(REF!D3,"0.0#")&amp;" Hz"))</f>
         <v>32.0 MHz</v>
       </c>
-      <c r="E3" s="5" t="str">
+      <c r="E3" s="2" t="str">
         <f>IF(REF!E3&gt;=10^6,TEXT(REF!E3/10^6,"0.0#")&amp;" MHz",IF(REF!E3&gt;=10^3,TEXT(REF!E3/10^3,"0.0#")&amp;" KHz",TEXT(REF!E3,"0.0#")&amp;" Hz"))</f>
         <v>16.0 MHz</v>
       </c>
-      <c r="F3" s="5" t="str">
+      <c r="F3" s="2" t="str">
         <f>IF(REF!F3&gt;=10^6,TEXT(REF!F3/10^6,"0.0#")&amp;" MHz",IF(REF!F3&gt;=10^3,TEXT(REF!F3/10^3,"0.0#")&amp;" KHz",TEXT(REF!F3,"0.0#")&amp;" Hz"))</f>
         <v>8.0 MHz</v>
       </c>
-      <c r="G3" s="5" t="str">
+      <c r="G3" s="2" t="str">
         <f>IF(REF!G3&gt;=10^6,TEXT(REF!G3/10^6,"0.0#")&amp;" MHz",IF(REF!G3&gt;=10^3,TEXT(REF!G3/10^3,"0.0#")&amp;" KHz",TEXT(REF!G3,"0.0#")&amp;" Hz"))</f>
         <v>4.0 MHz</v>
       </c>
-      <c r="H3" s="5" t="str">
+      <c r="H3" s="2" t="str">
         <f>IF(REF!H3&gt;=10^6,TEXT(REF!H3/10^6,"0.0#")&amp;" MHz",IF(REF!H3&gt;=10^3,TEXT(REF!H3/10^3,"0.0#")&amp;" KHz",TEXT(REF!H3,"0.0#")&amp;" Hz"))</f>
         <v>2.0 MHz</v>
       </c>
-      <c r="I3" s="5" t="str">
+      <c r="I3" s="2" t="str">
         <f>IF(REF!I3&gt;=10^6,TEXT(REF!I3/10^6,"0.0#")&amp;" MHz",IF(REF!I3&gt;=10^3,TEXT(REF!I3/10^3,"0.0#")&amp;" KHz",TEXT(REF!I3,"0.0#")&amp;" Hz"))</f>
         <v>1.0 MHz</v>
       </c>
-      <c r="J3" s="5" t="str">
+      <c r="J3" s="2" t="str">
         <f>IF(REF!J3&gt;=10^6,TEXT(REF!J3/10^6,"0.0#")&amp;" MHz",IF(REF!J3&gt;=10^3,TEXT(REF!J3/10^3,"0.0#")&amp;" KHz",TEXT(REF!J3,"0.0#")&amp;" Hz"))</f>
         <v>500.0 KHz</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="18" t="str">
+    <row r="4" spans="1:11" ht="42" customHeight="1">
+      <c r="A4" s="19"/>
+      <c r="B4" s="8" t="str">
         <f>IF(REF!B4&gt;=10^6,TEXT(REF!B4/10^6,"0.0#")&amp;" MHz",IF(REF!B4&gt;=10^3,TEXT(REF!B4/10^3,"0.0#")&amp;" KHz",TEXT(REF!B4,"0.0#")&amp;" Hz"))</f>
         <v>8.0 MHz</v>
       </c>
-      <c r="C4" s="5" t="str">
+      <c r="C4" s="2" t="str">
         <f>IF(REF!C4&gt;=10^6,TEXT(REF!C4/10^6,"0.0#")&amp;" MHz",IF(REF!C4&gt;=10^3,TEXT(REF!C4/10^3,"0.0#")&amp;" KHz",TEXT(REF!C4,"0.0#")&amp;" Hz"))</f>
         <v>128.0 MHz</v>
       </c>
-      <c r="D4" s="5" t="str">
+      <c r="D4" s="2" t="str">
         <f>IF(REF!D4&gt;=10^6,TEXT(REF!D4/10^6,"0.0#")&amp;" MHz",IF(REF!D4&gt;=10^3,TEXT(REF!D4/10^3,"0.0#")&amp;" KHz",TEXT(REF!D4,"0.0#")&amp;" Hz"))</f>
         <v>64.0 MHz</v>
       </c>
-      <c r="E4" s="5" t="str">
+      <c r="E4" s="2" t="str">
         <f>IF(REF!E4&gt;=10^6,TEXT(REF!E4/10^6,"0.0#")&amp;" MHz",IF(REF!E4&gt;=10^3,TEXT(REF!E4/10^3,"0.0#")&amp;" KHz",TEXT(REF!E4,"0.0#")&amp;" Hz"))</f>
         <v>32.0 MHz</v>
       </c>
-      <c r="F4" s="5" t="str">
+      <c r="F4" s="2" t="str">
         <f>IF(REF!F4&gt;=10^6,TEXT(REF!F4/10^6,"0.0#")&amp;" MHz",IF(REF!F4&gt;=10^3,TEXT(REF!F4/10^3,"0.0#")&amp;" KHz",TEXT(REF!F4,"0.0#")&amp;" Hz"))</f>
         <v>16.0 MHz</v>
       </c>
-      <c r="G4" s="5" t="str">
+      <c r="G4" s="2" t="str">
         <f>IF(REF!G4&gt;=10^6,TEXT(REF!G4/10^6,"0.0#")&amp;" MHz",IF(REF!G4&gt;=10^3,TEXT(REF!G4/10^3,"0.0#")&amp;" KHz",TEXT(REF!G4,"0.0#")&amp;" Hz"))</f>
         <v>8.0 MHz</v>
       </c>
-      <c r="H4" s="5" t="str">
+      <c r="H4" s="2" t="str">
         <f>IF(REF!H4&gt;=10^6,TEXT(REF!H4/10^6,"0.0#")&amp;" MHz",IF(REF!H4&gt;=10^3,TEXT(REF!H4/10^3,"0.0#")&amp;" KHz",TEXT(REF!H4,"0.0#")&amp;" Hz"))</f>
         <v>4.0 MHz</v>
       </c>
-      <c r="I4" s="5" t="str">
+      <c r="I4" s="2" t="str">
         <f>IF(REF!I4&gt;=10^6,TEXT(REF!I4/10^6,"0.0#")&amp;" MHz",IF(REF!I4&gt;=10^3,TEXT(REF!I4/10^3,"0.0#")&amp;" KHz",TEXT(REF!I4,"0.0#")&amp;" Hz"))</f>
         <v>2.0 MHz</v>
       </c>
-      <c r="J4" s="5" t="str">
+      <c r="J4" s="2" t="str">
         <f>IF(REF!J4&gt;=10^6,TEXT(REF!J4/10^6,"0.0#")&amp;" MHz",IF(REF!J4&gt;=10^3,TEXT(REF!J4/10^3,"0.0#")&amp;" KHz",TEXT(REF!J4,"0.0#")&amp;" Hz"))</f>
         <v>1.0 MHz</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="13" t="s">
+    <row r="5" spans="1:11">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" ht="45">
+      <c r="A6" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6">
-        <v>75575000</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="14" t="s">
+      <c r="B6" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="28">
+        <v>100000000</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8">
+    </row>
+    <row r="7" spans="1:11" ht="30">
+      <c r="A7" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="29">
         <f>80*POWER(10,6)</f>
         <v>80000000</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="31">
+      <c r="D7" s="29"/>
+      <c r="E7" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="17">
         <f>IF(AND(C6&lt;=REF!C4,C6&gt;=REF!C3),1,IF(AND(C6&lt;=REF!D4,C6&gt;=REF!D3),1/2,IF(AND(C6&lt;=REF!E4,C6&gt;=REF!E3),1/4,IF(AND(C6&lt;=REF!F4,C6&gt;=REF!F3),1/8,IF(AND(C6&lt;=REF!G4,C6&gt;=REF!G3),1/16,IF(AND(C6&lt;=REF!H4,C6&gt;=REF!H3),1/32,IF(AND(C6&lt;=REF!I4,C6&gt;=REF!I3),1/64,IF(AND(C6&lt;=REF!J4,C6&gt;=REF!J3),1/128,0))))))))</f>
         <v>1</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="22">
+      <c r="D8" s="3"/>
+      <c r="E8" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="23"/>
+      <c r="B9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="21">
         <f>ROUND((C6*POWER(2,32))/(16*C8*C7),0)</f>
-        <v>253587620</v>
-      </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="28" t="s">
+        <v>335544320</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="25" t="str">
+    <row r="10" spans="1:11">
+      <c r="A10" s="23"/>
+      <c r="B10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="22" t="str">
         <f>DEC2BIN((MOD(C9,4294967296)/16777216),8)&amp;DEC2BIN(MOD(C9,16777216)/65536,8)&amp;DEC2BIN(MOD(C9,65536)/256,8)&amp;DEC2BIN(MOD(C9,256),8)</f>
-        <v>00001111000111010111000010100100</v>
-      </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="29" t="s">
+        <v>00010100000000000000000000000000</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="23"/>
+      <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="24" t="str">
+      <c r="C11" s="18" t="str">
         <f>DEC2HEX(C9)</f>
-        <v>F1D70A4</v>
-      </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="12" t="str">
-        <f>IF(REF!B6&gt;=10^6,TEXT(REF!B6/10^6,"0.0#"),IF(REF!B6&gt;=10^3,TEXT(REF!B63/10^3,"0.0#"),TEXT(REF!B6,"0.0#")))</f>
-        <v>4.72</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="26" t="str">
-        <f>IF(REF!B6&gt;=10^6," MHz",IF(REF!B6&gt;=10^3," KHz"," Hz"))</f>
-        <v xml:space="preserve"> MHz</v>
+        <v>14000000</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="C11:E11"/>
-    <mergeCell ref="A6:A12"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:E10"/>
+    <mergeCell ref="A8:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="207" yWindow="407" count="1">
-        <x14:dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="PLL_out Range" error="PLL_out must between 500 kHz and 128 MHz" promptTitle="PLL_out Range" prompt="PLL_out must between 500 kHz and 128 MHz">
+        <x14:dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="PLL_out Range" error="PLL_out must between 500 kHz and 128 MHz" promptTitle="PLL_out Range" prompt="PLL_out must between 500 kHz and 128 MHz" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>AND(C6&gt;=REF!J3,C6&lt;=REF!C4)</xm:f>
           </x14:formula1>
@@ -1038,19 +1036,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10">
       <c r="C2">
         <v>1</v>
       </c>
@@ -1076,7 +1074,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10">
       <c r="B3">
         <v>4000000</v>
       </c>
@@ -1113,7 +1111,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="B4">
         <v>8000000</v>
       </c>
@@ -1150,10 +1148,10 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="B6">
         <f>ROUND(('Counter PLL Calc'!C9*'Counter PLL Calc'!C7)/POWER(2,32),0)</f>
-        <v>4723438</v>
+        <v>6250000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More tinkering with vga.spin. Updated counter PLL calc.
</commit_message>
<xml_diff>
--- a/Docs/Other/Counter_PLL_Calc.xlsx
+++ b/Docs/Other/Counter_PLL_Calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unkno\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04D44088-EFB9-4879-922C-E7518C8E3E94}" xr6:coauthVersionLast="20" xr6:coauthVersionMax="20" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{028C8D86-3CE1-4674-B5F2-5E8F829BC603}" xr6:coauthVersionLast="20" xr6:coauthVersionMax="20" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>PLLDIV dividers</t>
   </si>
@@ -82,16 +82,19 @@
     <t>x VCO</t>
   </si>
   <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>(binary)</t>
+  </si>
+  <si>
+    <t>(dec/hex)</t>
+  </si>
+  <si>
     <t>FRQX =</t>
   </si>
   <si>
     <t>(decimal)</t>
-  </si>
-  <si>
-    <t>=</t>
-  </si>
-  <si>
-    <t>(binary)</t>
   </si>
   <si>
     <t>(hex)</t>
@@ -142,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +176,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6D9F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD7E3BC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -299,12 +314,80 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -313,9 +396,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -326,79 +407,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -411,85 +420,89 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -771,16 +784,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -795,148 +809,148 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="B1" s="1"/>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1"/>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="43.5" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7" t="str">
+      <c r="B3" s="4" t="str">
+        <f>IF(REF!A2&gt;=10^6,TEXT(REF!A2/10^6,"0.0#")&amp;" MHz",IF(REF!A2&gt;=10^3,TEXT(REF!A2/10^3,"0.0#")&amp;" KHz",TEXT(REF!A2,"0.0#")&amp;" Hz"))</f>
+        <v>4.0 MHz</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f>IF(REF!B2&gt;=10^6,TEXT(REF!B2/10^6,"0.0#")&amp;" MHz",IF(REF!B2&gt;=10^3,TEXT(REF!B2/10^3,"0.0#")&amp;" KHz",TEXT(REF!B2,"0.0#")&amp;" Hz"))</f>
+        <v>64.0 MHz</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f>IF(REF!C2&gt;=10^6,TEXT(REF!C2/10^6,"0.0#")&amp;" MHz",IF(REF!C2&gt;=10^3,TEXT(REF!C2/10^3,"0.0#")&amp;" KHz",TEXT(REF!C2,"0.0#")&amp;" Hz"))</f>
+        <v>32.0 MHz</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f>IF(REF!D2&gt;=10^6,TEXT(REF!D2/10^6,"0.0#")&amp;" MHz",IF(REF!D2&gt;=10^3,TEXT(REF!D2/10^3,"0.0#")&amp;" KHz",TEXT(REF!D2,"0.0#")&amp;" Hz"))</f>
+        <v>16.0 MHz</v>
+      </c>
+      <c r="F3" s="2" t="str">
+        <f>IF(REF!E2&gt;=10^6,TEXT(REF!E2/10^6,"0.0#")&amp;" MHz",IF(REF!E2&gt;=10^3,TEXT(REF!E2/10^3,"0.0#")&amp;" KHz",TEXT(REF!E2,"0.0#")&amp;" Hz"))</f>
+        <v>8.0 MHz</v>
+      </c>
+      <c r="G3" s="2" t="str">
+        <f>IF(REF!F2&gt;=10^6,TEXT(REF!F2/10^6,"0.0#")&amp;" MHz",IF(REF!F2&gt;=10^3,TEXT(REF!F2/10^3,"0.0#")&amp;" KHz",TEXT(REF!F2,"0.0#")&amp;" Hz"))</f>
+        <v>4.0 MHz</v>
+      </c>
+      <c r="H3" s="2" t="str">
+        <f>IF(REF!G2&gt;=10^6,TEXT(REF!G2/10^6,"0.0#")&amp;" MHz",IF(REF!G2&gt;=10^3,TEXT(REF!G2/10^3,"0.0#")&amp;" KHz",TEXT(REF!G2,"0.0#")&amp;" Hz"))</f>
+        <v>2.0 MHz</v>
+      </c>
+      <c r="I3" s="2" t="str">
+        <f>IF(REF!H2&gt;=10^6,TEXT(REF!H2/10^6,"0.0#")&amp;" MHz",IF(REF!H2&gt;=10^3,TEXT(REF!H2/10^3,"0.0#")&amp;" KHz",TEXT(REF!H2,"0.0#")&amp;" Hz"))</f>
+        <v>1.0 MHz</v>
+      </c>
+      <c r="J3" s="2" t="str">
+        <f>IF(REF!I2&gt;=10^6,TEXT(REF!I2/10^6,"0.0#")&amp;" MHz",IF(REF!I2&gt;=10^3,TEXT(REF!I2/10^3,"0.0#")&amp;" KHz",TEXT(REF!I2,"0.0#")&amp;" Hz"))</f>
+        <v>500.0 KHz</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="42" customHeight="1">
+      <c r="A4" s="20"/>
+      <c r="B4" s="5" t="str">
+        <f>IF(REF!A3&gt;=10^6,TEXT(REF!A3/10^6,"0.0#")&amp;" MHz",IF(REF!A3&gt;=10^3,TEXT(REF!A3/10^3,"0.0#")&amp;" KHz",TEXT(REF!A3,"0.0#")&amp;" Hz"))</f>
+        <v>8.0 MHz</v>
+      </c>
+      <c r="C4" s="2" t="str">
         <f>IF(REF!B3&gt;=10^6,TEXT(REF!B3/10^6,"0.0#")&amp;" MHz",IF(REF!B3&gt;=10^3,TEXT(REF!B3/10^3,"0.0#")&amp;" KHz",TEXT(REF!B3,"0.0#")&amp;" Hz"))</f>
-        <v>4.0 MHz</v>
-      </c>
-      <c r="C3" s="2" t="str">
+        <v>128.0 MHz</v>
+      </c>
+      <c r="D4" s="2" t="str">
         <f>IF(REF!C3&gt;=10^6,TEXT(REF!C3/10^6,"0.0#")&amp;" MHz",IF(REF!C3&gt;=10^3,TEXT(REF!C3/10^3,"0.0#")&amp;" KHz",TEXT(REF!C3,"0.0#")&amp;" Hz"))</f>
         <v>64.0 MHz</v>
       </c>
-      <c r="D3" s="2" t="str">
+      <c r="E4" s="2" t="str">
         <f>IF(REF!D3&gt;=10^6,TEXT(REF!D3/10^6,"0.0#")&amp;" MHz",IF(REF!D3&gt;=10^3,TEXT(REF!D3/10^3,"0.0#")&amp;" KHz",TEXT(REF!D3,"0.0#")&amp;" Hz"))</f>
         <v>32.0 MHz</v>
       </c>
-      <c r="E3" s="2" t="str">
+      <c r="F4" s="2" t="str">
         <f>IF(REF!E3&gt;=10^6,TEXT(REF!E3/10^6,"0.0#")&amp;" MHz",IF(REF!E3&gt;=10^3,TEXT(REF!E3/10^3,"0.0#")&amp;" KHz",TEXT(REF!E3,"0.0#")&amp;" Hz"))</f>
         <v>16.0 MHz</v>
       </c>
-      <c r="F3" s="2" t="str">
+      <c r="G4" s="2" t="str">
         <f>IF(REF!F3&gt;=10^6,TEXT(REF!F3/10^6,"0.0#")&amp;" MHz",IF(REF!F3&gt;=10^3,TEXT(REF!F3/10^3,"0.0#")&amp;" KHz",TEXT(REF!F3,"0.0#")&amp;" Hz"))</f>
         <v>8.0 MHz</v>
       </c>
-      <c r="G3" s="2" t="str">
+      <c r="H4" s="2" t="str">
         <f>IF(REF!G3&gt;=10^6,TEXT(REF!G3/10^6,"0.0#")&amp;" MHz",IF(REF!G3&gt;=10^3,TEXT(REF!G3/10^3,"0.0#")&amp;" KHz",TEXT(REF!G3,"0.0#")&amp;" Hz"))</f>
         <v>4.0 MHz</v>
       </c>
-      <c r="H3" s="2" t="str">
+      <c r="I4" s="2" t="str">
         <f>IF(REF!H3&gt;=10^6,TEXT(REF!H3/10^6,"0.0#")&amp;" MHz",IF(REF!H3&gt;=10^3,TEXT(REF!H3/10^3,"0.0#")&amp;" KHz",TEXT(REF!H3,"0.0#")&amp;" Hz"))</f>
         <v>2.0 MHz</v>
       </c>
-      <c r="I3" s="2" t="str">
+      <c r="J4" s="2" t="str">
         <f>IF(REF!I3&gt;=10^6,TEXT(REF!I3/10^6,"0.0#")&amp;" MHz",IF(REF!I3&gt;=10^3,TEXT(REF!I3/10^3,"0.0#")&amp;" KHz",TEXT(REF!I3,"0.0#")&amp;" Hz"))</f>
         <v>1.0 MHz</v>
       </c>
-      <c r="J3" s="2" t="str">
-        <f>IF(REF!J3&gt;=10^6,TEXT(REF!J3/10^6,"0.0#")&amp;" MHz",IF(REF!J3&gt;=10^3,TEXT(REF!J3/10^3,"0.0#")&amp;" KHz",TEXT(REF!J3,"0.0#")&amp;" Hz"))</f>
-        <v>500.0 KHz</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="19"/>
-      <c r="B4" s="8" t="str">
-        <f>IF(REF!B4&gt;=10^6,TEXT(REF!B4/10^6,"0.0#")&amp;" MHz",IF(REF!B4&gt;=10^3,TEXT(REF!B4/10^3,"0.0#")&amp;" KHz",TEXT(REF!B4,"0.0#")&amp;" Hz"))</f>
-        <v>8.0 MHz</v>
-      </c>
-      <c r="C4" s="2" t="str">
-        <f>IF(REF!C4&gt;=10^6,TEXT(REF!C4/10^6,"0.0#")&amp;" MHz",IF(REF!C4&gt;=10^3,TEXT(REF!C4/10^3,"0.0#")&amp;" KHz",TEXT(REF!C4,"0.0#")&amp;" Hz"))</f>
-        <v>128.0 MHz</v>
-      </c>
-      <c r="D4" s="2" t="str">
-        <f>IF(REF!D4&gt;=10^6,TEXT(REF!D4/10^6,"0.0#")&amp;" MHz",IF(REF!D4&gt;=10^3,TEXT(REF!D4/10^3,"0.0#")&amp;" KHz",TEXT(REF!D4,"0.0#")&amp;" Hz"))</f>
-        <v>64.0 MHz</v>
-      </c>
-      <c r="E4" s="2" t="str">
-        <f>IF(REF!E4&gt;=10^6,TEXT(REF!E4/10^6,"0.0#")&amp;" MHz",IF(REF!E4&gt;=10^3,TEXT(REF!E4/10^3,"0.0#")&amp;" KHz",TEXT(REF!E4,"0.0#")&amp;" Hz"))</f>
-        <v>32.0 MHz</v>
-      </c>
-      <c r="F4" s="2" t="str">
-        <f>IF(REF!F4&gt;=10^6,TEXT(REF!F4/10^6,"0.0#")&amp;" MHz",IF(REF!F4&gt;=10^3,TEXT(REF!F4/10^3,"0.0#")&amp;" KHz",TEXT(REF!F4,"0.0#")&amp;" Hz"))</f>
-        <v>16.0 MHz</v>
-      </c>
-      <c r="G4" s="2" t="str">
-        <f>IF(REF!G4&gt;=10^6,TEXT(REF!G4/10^6,"0.0#")&amp;" MHz",IF(REF!G4&gt;=10^3,TEXT(REF!G4/10^3,"0.0#")&amp;" KHz",TEXT(REF!G4,"0.0#")&amp;" Hz"))</f>
-        <v>8.0 MHz</v>
-      </c>
-      <c r="H4" s="2" t="str">
-        <f>IF(REF!H4&gt;=10^6,TEXT(REF!H4/10^6,"0.0#")&amp;" MHz",IF(REF!H4&gt;=10^3,TEXT(REF!H4/10^3,"0.0#")&amp;" KHz",TEXT(REF!H4,"0.0#")&amp;" Hz"))</f>
-        <v>4.0 MHz</v>
-      </c>
-      <c r="I4" s="2" t="str">
-        <f>IF(REF!I4&gt;=10^6,TEXT(REF!I4/10^6,"0.0#")&amp;" MHz",IF(REF!I4&gt;=10^3,TEXT(REF!I4/10^3,"0.0#")&amp;" KHz",TEXT(REF!I4,"0.0#")&amp;" Hz"))</f>
-        <v>2.0 MHz</v>
-      </c>
-      <c r="J4" s="2" t="str">
-        <f>IF(REF!J4&gt;=10^6,TEXT(REF!J4/10^6,"0.0#")&amp;" MHz",IF(REF!J4&gt;=10^3,TEXT(REF!J4/10^3,"0.0#")&amp;" KHz",TEXT(REF!J4,"0.0#")&amp;" Hz"))</f>
-        <v>1.0 MHz</v>
-      </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:11" ht="45">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="28">
-        <v>100000000</v>
-      </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="25" t="s">
+      <c r="C6" s="30">
+        <v>20000000</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="30">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:11" ht="44.25" customHeight="1">
+      <c r="A7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="29">
@@ -944,79 +958,112 @@
         <v>80000000</v>
       </c>
       <c r="D7" s="29"/>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="17">
-        <f>IF(AND(C6&lt;=REF!C4,C6&gt;=REF!C3),1,IF(AND(C6&lt;=REF!D4,C6&gt;=REF!D3),1/2,IF(AND(C6&lt;=REF!E4,C6&gt;=REF!E3),1/4,IF(AND(C6&lt;=REF!F4,C6&gt;=REF!F3),1/8,IF(AND(C6&lt;=REF!G4,C6&gt;=REF!G3),1/16,IF(AND(C6&lt;=REF!H4,C6&gt;=REF!H3),1/32,IF(AND(C6&lt;=REF!I4,C6&gt;=REF!I3),1/64,IF(AND(C6&lt;=REF!J4,C6&gt;=REF!J3),1/128,0))))))))</f>
-        <v>1</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4" t="s">
+      <c r="C8" s="28">
+        <f>IF(AND(C6&lt;=REF!B3,C6&gt;=REF!B2),1,IF(AND(C6&lt;=REF!C3,C6&gt;=REF!C2),1/2,IF(AND(C6&lt;=REF!D3,C6&gt;=REF!D2),1/4,IF(AND(C6&lt;=REF!E3,C6&gt;=REF!E2),1/8,IF(AND(C6&lt;=REF!F3,C6&gt;=REF!F2),1/16,IF(AND(C6&lt;=REF!G3,C6&gt;=REF!G2),1/32,IF(AND(C6&lt;=REF!H3,C6&gt;=REF!H2),1/64,IF(AND(C6&lt;=REF!I3,C6&gt;=REF!I2),1/128,0))))))))</f>
+        <v>0.25</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="23"/>
-      <c r="B9" s="12" t="s">
+      <c r="A9" s="25"/>
+      <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="27" t="str">
+        <f>IF(AND(C6&lt;=REF!B3,C6&gt;=REF!B2),"111",IF(AND(C6&lt;=REF!C3,C6&gt;=REF!C2),"110",IF(AND(C6&lt;=REF!D3,C6&gt;=REF!D2),"101",IF(AND(C6&lt;=REF!E3,C6&gt;=REF!E2),"100",IF(AND(C6&lt;=REF!F3,C6&gt;=REF!F2),"011",IF(AND(C6&lt;=REF!G3,C6&gt;=REF!G2),"010",IF(AND(C6&lt;=REF!H3,C6&gt;=REF!H2),"001",IF(AND(C6&lt;=REF!I3,C6&gt;=REF!I2),"000",0))))))))</f>
+        <v>101</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="25"/>
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="22" t="str">
+        <f>BIN2HEX(C9)</f>
+        <v>5</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="25"/>
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="23">
         <f>ROUND((C6*POWER(2,32))/(16*C8*C7),0)</f>
-        <v>335544320</v>
-      </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14" t="s">
+        <v>268435456</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="25"/>
+      <c r="B12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="23" t="str">
+        <f>DEC2BIN((MOD(C11,4294967296)/16777216),8)&amp;DEC2BIN(MOD(C11,16777216)/65536,8)&amp;DEC2BIN(MOD(C11,65536)/256,8)&amp;DEC2BIN(MOD(C11,256),8)</f>
+        <v>00010000000000000000000000000000</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="23"/>
-      <c r="B10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="22" t="str">
-        <f>DEC2BIN((MOD(C9,4294967296)/16777216),8)&amp;DEC2BIN(MOD(C9,16777216)/65536,8)&amp;DEC2BIN(MOD(C9,65536)/256,8)&amp;DEC2BIN(MOD(C9,256),8)</f>
-        <v>00010100000000000000000000000000</v>
-      </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="23"/>
-      <c r="B11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="18" t="str">
-        <f>DEC2HEX(C9)</f>
-        <v>14000000</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="16" t="s">
-        <v>22</v>
+    <row r="13" spans="1:11">
+      <c r="A13" s="25"/>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="26" t="str">
+        <f>DEC2HEX(C11)</f>
+        <v>10000000</v>
+      </c>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="19" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C11:E11"/>
+  <mergeCells count="11">
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="C13:E13"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1025,7 +1072,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="207" yWindow="407" count="1">
         <x14:dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="PLL_out Range" error="PLL_out must between 500 kHz and 128 MHz" promptTitle="PLL_out Range" prompt="PLL_out must between 500 kHz and 128 MHz" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
-            <xm:f>AND(C6&gt;=REF!J3,C6&lt;=REF!C4)</xm:f>
+            <xm:f>AND(C6&gt;=REF!I2,C6&lt;=REF!B3)</xm:f>
           </x14:formula1>
           <xm:sqref>C6</xm:sqref>
         </x14:dataValidation>
@@ -1037,10 +1084,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:J6"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1048,110 +1095,110 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="1" spans="1:9">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <v>16</v>
+      </c>
+      <c r="G1">
+        <v>32</v>
+      </c>
+      <c r="H1">
+        <v>64</v>
+      </c>
+      <c r="I1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>4000000</v>
+      </c>
+      <c r="B2">
+        <f>($A$2*16)/B1</f>
+        <v>64000000</v>
+      </c>
       <c r="C2">
-        <v>1</v>
+        <f>($A$2*16)/C1</f>
+        <v>32000000</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <f>($A$2*16)/D1</f>
+        <v>16000000</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <f>($A$2*16)/E1</f>
+        <v>8000000</v>
       </c>
       <c r="F2">
-        <v>8</v>
+        <f>($A$2*16)/F1</f>
+        <v>4000000</v>
       </c>
       <c r="G2">
-        <v>16</v>
+        <f>($A$2*16)/G1</f>
+        <v>2000000</v>
       </c>
       <c r="H2">
-        <v>32</v>
+        <f>($A$2*16)/H1</f>
+        <v>1000000</v>
       </c>
       <c r="I2">
-        <v>64</v>
-      </c>
-      <c r="J2">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10">
+        <f>($A$2*16)/I1</f>
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>8000000</v>
+      </c>
       <c r="B3">
+        <f>($A$3*16)/B1</f>
+        <v>128000000</v>
+      </c>
+      <c r="C3">
+        <f>($A$3*16)/C1</f>
+        <v>64000000</v>
+      </c>
+      <c r="D3">
+        <f>($A$3*16)/D1</f>
+        <v>32000000</v>
+      </c>
+      <c r="E3">
+        <f>($A$3*16)/E1</f>
+        <v>16000000</v>
+      </c>
+      <c r="F3">
+        <f>($A$3*16)/F1</f>
+        <v>8000000</v>
+      </c>
+      <c r="G3">
+        <f>($A$3*16)/G1</f>
         <v>4000000</v>
       </c>
-      <c r="C3">
-        <f>($B$3*16)/C2</f>
-        <v>64000000</v>
-      </c>
-      <c r="D3">
-        <f>($B$3*16)/D2</f>
-        <v>32000000</v>
-      </c>
-      <c r="E3">
-        <f>($B$3*16)/E2</f>
-        <v>16000000</v>
-      </c>
-      <c r="F3">
-        <f>($B$3*16)/F2</f>
-        <v>8000000</v>
-      </c>
-      <c r="G3">
-        <f>($B$3*16)/G2</f>
-        <v>4000000</v>
-      </c>
       <c r="H3">
-        <f>($B$3*16)/H2</f>
+        <f>($A$3*16)/H1</f>
         <v>2000000</v>
       </c>
       <c r="I3">
-        <f>($B$3*16)/I2</f>
+        <f>($A$3*16)/I1</f>
         <v>1000000</v>
       </c>
-      <c r="J3">
-        <f>($B$3*16)/J2</f>
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10">
-      <c r="B4">
-        <v>8000000</v>
-      </c>
-      <c r="C4">
-        <f>($B$4*16)/C2</f>
-        <v>128000000</v>
-      </c>
-      <c r="D4">
-        <f>($B$4*16)/D2</f>
-        <v>64000000</v>
-      </c>
-      <c r="E4">
-        <f>($B$4*16)/E2</f>
-        <v>32000000</v>
-      </c>
-      <c r="F4">
-        <f>($B$4*16)/F2</f>
-        <v>16000000</v>
-      </c>
-      <c r="G4">
-        <f>($B$4*16)/G2</f>
-        <v>8000000</v>
-      </c>
-      <c r="H4">
-        <f>($B$4*16)/H2</f>
-        <v>4000000</v>
-      </c>
-      <c r="I4">
-        <f>($B$4*16)/I2</f>
-        <v>2000000</v>
-      </c>
-      <c r="J4">
-        <f>($B$4*16)/J2</f>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="B6">
-        <f>ROUND(('Counter PLL Calc'!C9*'Counter PLL Calc'!C7)/POWER(2,32),0)</f>
-        <v>6250000</v>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <f>ROUND(('Counter PLL Calc'!C11*'Counter PLL Calc'!C7)/POWER(2,32),0)</f>
+        <v>5000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Began adding video generation logic to vga.spin. Populated counter PLL calculator w/ 640x480 @ 60 Hz values.
</commit_message>
<xml_diff>
--- a/Docs/Other/Counter_PLL_Calc.xlsx
+++ b/Docs/Other/Counter_PLL_Calc.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unkno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\JCAP\Docs\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{028C8D86-3CE1-4674-B5F2-5E8F829BC603}" xr6:coauthVersionLast="20" xr6:coauthVersionMax="20" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18420"/>
   </bookViews>
   <sheets>
     <sheet name="Counter PLL Calc" sheetId="1" r:id="rId1"/>
     <sheet name="REF" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -103,11 +102,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#\ ???/???"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -783,14 +782,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -807,7 +806,7 @@
     <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="21" t="s">
         <v>0</v>
@@ -821,7 +820,7 @@
       <c r="J1" s="21"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="C2" s="15" t="s">
         <v>1</v>
@@ -848,7 +847,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="43.5" customHeight="1">
+    <row r="3" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>9</v>
       </c>
@@ -889,7 +888,7 @@
         <v>500.0 KHz</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="42" customHeight="1">
+    <row r="4" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20"/>
       <c r="B4" s="5" t="str">
         <f>IF(REF!A3&gt;=10^6,TEXT(REF!A3/10^6,"0.0#")&amp;" MHz",IF(REF!A3&gt;=10^3,TEXT(REF!A3/10^3,"0.0#")&amp;" KHz",TEXT(REF!A3,"0.0#")&amp;" Hz"))</f>
@@ -928,10 +927,10 @@
         <v>1.0 MHz</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="45">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>10</v>
       </c>
@@ -939,14 +938,14 @@
         <v>11</v>
       </c>
       <c r="C6" s="30">
-        <v>20000000</v>
+        <v>25175000</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="44.25" customHeight="1">
+    <row r="7" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>13</v>
       </c>
@@ -962,7 +961,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>15</v>
       </c>
@@ -978,7 +977,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
       <c r="B9" s="6" t="s">
         <v>18</v>
@@ -992,7 +991,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
       <c r="B10" s="6" t="s">
         <v>18</v>
@@ -1006,14 +1005,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
       <c r="B11" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="23">
         <f>ROUND((C6*POWER(2,32))/(16*C8*C7),0)</f>
-        <v>268435456</v>
+        <v>337893130</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
@@ -1021,14 +1020,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
       <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="23" t="str">
         <f>DEC2BIN((MOD(C11,4294967296)/16777216),8)&amp;DEC2BIN(MOD(C11,16777216)/65536,8)&amp;DEC2BIN(MOD(C11,65536)/256,8)&amp;DEC2BIN(MOD(C11,256),8)</f>
-        <v>00010000000000000000000000000000</v>
+        <v>00010100001000111101011100001010</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -1036,14 +1035,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
       <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="26" t="str">
         <f>DEC2HEX(C11)</f>
-        <v>10000000</v>
+        <v>1423D70A</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
@@ -1070,7 +1069,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="207" yWindow="407" count="1">
-        <x14:dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="PLL_out Range" error="PLL_out must between 500 kHz and 128 MHz" promptTitle="PLL_out Range" prompt="PLL_out must between 500 kHz and 128 MHz" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="PLL_out Range" error="PLL_out must between 500 kHz and 128 MHz" promptTitle="PLL_out Range" prompt="PLL_out must between 500 kHz and 128 MHz">
           <x14:formula1>
             <xm:f>AND(C6&gt;=REF!I2,C6&lt;=REF!B3)</xm:f>
           </x14:formula1>
@@ -1083,19 +1082,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>1</v>
       </c>
@@ -1121,84 +1120,84 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4000000</v>
       </c>
       <c r="B2">
-        <f>($A$2*16)/B1</f>
+        <f t="shared" ref="B2:I2" si="0">($A$2*16)/B1</f>
         <v>64000000</v>
       </c>
       <c r="C2">
-        <f>($A$2*16)/C1</f>
+        <f t="shared" si="0"/>
         <v>32000000</v>
       </c>
       <c r="D2">
-        <f>($A$2*16)/D1</f>
+        <f t="shared" si="0"/>
         <v>16000000</v>
       </c>
       <c r="E2">
-        <f>($A$2*16)/E1</f>
+        <f t="shared" si="0"/>
         <v>8000000</v>
       </c>
       <c r="F2">
-        <f>($A$2*16)/F1</f>
+        <f t="shared" si="0"/>
         <v>4000000</v>
       </c>
       <c r="G2">
-        <f>($A$2*16)/G1</f>
+        <f t="shared" si="0"/>
         <v>2000000</v>
       </c>
       <c r="H2">
-        <f>($A$2*16)/H1</f>
+        <f t="shared" si="0"/>
         <v>1000000</v>
       </c>
       <c r="I2">
-        <f>($A$2*16)/I1</f>
+        <f t="shared" si="0"/>
         <v>500000</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8000000</v>
       </c>
       <c r="B3">
-        <f>($A$3*16)/B1</f>
+        <f t="shared" ref="B3:I3" si="1">($A$3*16)/B1</f>
         <v>128000000</v>
       </c>
       <c r="C3">
-        <f>($A$3*16)/C1</f>
+        <f t="shared" si="1"/>
         <v>64000000</v>
       </c>
       <c r="D3">
-        <f>($A$3*16)/D1</f>
+        <f t="shared" si="1"/>
         <v>32000000</v>
       </c>
       <c r="E3">
-        <f>($A$3*16)/E1</f>
+        <f t="shared" si="1"/>
         <v>16000000</v>
       </c>
       <c r="F3">
-        <f>($A$3*16)/F1</f>
+        <f t="shared" si="1"/>
         <v>8000000</v>
       </c>
       <c r="G3">
-        <f>($A$3*16)/G1</f>
+        <f t="shared" si="1"/>
         <v>4000000</v>
       </c>
       <c r="H3">
-        <f>($A$3*16)/H1</f>
+        <f t="shared" si="1"/>
         <v>2000000</v>
       </c>
       <c r="I3">
-        <f>($A$3*16)/I1</f>
+        <f t="shared" si="1"/>
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>ROUND(('Counter PLL Calc'!C11*'Counter PLL Calc'!C7)/POWER(2,32),0)</f>
-        <v>5000000</v>
+        <v>6293750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed basic sprite system; removed redundant documents
</commit_message>
<xml_diff>
--- a/Docs/Other/Counter_PLL_Calc.xlsx
+++ b/Docs/Other/Counter_PLL_Calc.xlsx
@@ -786,7 +786,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:D7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,8 +953,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="29">
-        <f>80*POWER(10,6)</f>
-        <v>80000000</v>
+        <v>104000000</v>
       </c>
       <c r="D7" s="29"/>
       <c r="E7" s="11" t="s">
@@ -1012,7 +1011,7 @@
       </c>
       <c r="C11" s="23">
         <f>ROUND((C6*POWER(2,32))/(16*C8*C7),0)</f>
-        <v>337893130</v>
+        <v>259917792</v>
       </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
@@ -1027,7 +1026,7 @@
       </c>
       <c r="C12" s="23" t="str">
         <f>DEC2BIN((MOD(C11,4294967296)/16777216),8)&amp;DEC2BIN(MOD(C11,16777216)/65536,8)&amp;DEC2BIN(MOD(C11,65536)/256,8)&amp;DEC2BIN(MOD(C11,256),8)</f>
-        <v>00010100001000111101011100001010</v>
+        <v>00001111011111100000011111100000</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -1042,7 +1041,7 @@
       </c>
       <c r="C13" s="26" t="str">
         <f>DEC2HEX(C11)</f>
-        <v>1423D70A</v>
+        <v>F7E07E0</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>

</xml_diff>